<commit_message>
made changes for #21
</commit_message>
<xml_diff>
--- a/docassemble/DivorceNoKids/data/sources/courts_list.xlsx
+++ b/docassemble/DivorceNoKids/data/sources/courts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miabonardi/Documents/Lemma Legal/Clients/LSV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stavrosconstantinou/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D71B47C0-DB31-304F-A515-17D940099F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6777630C-C40F-2D4F-A762-3D533B280DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -321,15 +321,54 @@
   </si>
   <si>
     <t>arbitrary_attribute (mailing address if different from street address)</t>
+  </si>
+  <si>
+    <t>"'05753"</t>
+  </si>
+  <si>
+    <t>"05201"</t>
+  </si>
+  <si>
+    <t>"05819"</t>
+  </si>
+  <si>
+    <t>"05401"</t>
+  </si>
+  <si>
+    <t>"05905"</t>
+  </si>
+  <si>
+    <t>"05478"</t>
+  </si>
+  <si>
+    <t>"05474"</t>
+  </si>
+  <si>
+    <t>"05655"</t>
+  </si>
+  <si>
+    <t>"05038"</t>
+  </si>
+  <si>
+    <t>"05855"</t>
+  </si>
+  <si>
+    <t>"05701"</t>
+  </si>
+  <si>
+    <t>"05641"</t>
+  </si>
+  <si>
+    <t>"05301"</t>
+  </si>
+  <si>
+    <t>"05001"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="00000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -407,8 +446,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A491E8-E2DE-9A4E-A3B9-C224836C99FE}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,8 +876,8 @@
       <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5">
-        <v>5753</v>
+      <c r="M2" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -874,8 +917,8 @@
       <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="6">
-        <v>5201</v>
+      <c r="M3" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
@@ -918,8 +961,8 @@
       <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="6">
-        <v>5819</v>
+      <c r="M4" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
@@ -962,8 +1005,8 @@
       <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="6">
-        <v>5401</v>
+      <c r="M5" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="N5" t="s">
         <v>34</v>
@@ -1003,8 +1046,8 @@
       <c r="L6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="6">
-        <v>5905</v>
+      <c r="M6" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="N6" t="s">
         <v>35</v>
@@ -1041,8 +1084,8 @@
       <c r="L7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="6">
-        <v>5478</v>
+      <c r="M7" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="N7" t="s">
         <v>36</v>
@@ -1076,8 +1119,8 @@
       <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="6">
-        <v>5474</v>
+      <c r="M8" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="N8" t="s">
         <v>37</v>
@@ -1114,8 +1157,8 @@
       <c r="L9" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="6">
-        <v>5655</v>
+      <c r="M9" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="N9" t="s">
         <v>38</v>
@@ -1152,8 +1195,8 @@
       <c r="L10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="6">
-        <v>5038</v>
+      <c r="M10" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="N10" t="s">
         <v>39</v>
@@ -1190,8 +1233,8 @@
       <c r="L11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="6">
-        <v>5855</v>
+      <c r="M11" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="N11" t="s">
         <v>40</v>
@@ -1225,8 +1268,8 @@
       <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="6">
-        <v>5701</v>
+      <c r="M12" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="N12" t="s">
         <v>30</v>
@@ -1263,8 +1306,8 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="6">
-        <v>5641</v>
+      <c r="M13" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="N13" t="s">
         <v>41</v>
@@ -1301,8 +1344,8 @@
       <c r="L14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="6">
-        <v>5301</v>
+      <c r="M14" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="N14" t="s">
         <v>42</v>
@@ -1336,8 +1379,8 @@
       <c r="L15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="6">
-        <v>5001</v>
+      <c r="M15" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="N15" t="s">
         <v>43</v>

</xml_diff>